<commit_message>
listo creación de quickbooks
</commit_message>
<xml_diff>
--- a/files/productsQBO.xlsx
+++ b/files/productsQBO.xlsx
@@ -15,12 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>Hello</t>
+    <t>Qty</t>
   </si>
   <si>
-    <t>world!</t>
+    <t>nroPart</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Custom Design</t>
   </si>
 </sst>
 </file>
@@ -371,16 +380,26 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>